<commit_message>
New IM template mapped
</commit_message>
<xml_diff>
--- a/api/src/main/resources/Template_MI_2021_v1.9.1.xlsx
+++ b/api/src/main/resources/Template_MI_2021_v1.9.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11670" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="4.Relatório_Indicadores" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="414">
   <si>
     <t>REPÚBLICA DE MOÇAMBIQUE
 MINISTÉRIO DA SAÚDE
@@ -2686,6 +2686,14 @@
   </si>
   <si>
     <t>Crianças (0-14) 
+   11.7</t>
+  </si>
+  <si>
+    <t>Mulher Grávida
+ 11.4</t>
+  </si>
+  <si>
+    <t>Crianças (0-14) 
    11.4</t>
   </si>
   <si>
@@ -2849,7 +2857,190 @@
 15.3</t>
   </si>
   <si>
+    <t>#IM.DRD#</t>
+  </si>
+  <si>
+    <t>#location#</t>
+  </si>
+  <si>
+    <t>#IM.IM7DENT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM7NUMT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM7DENT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM7NUMT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM11DENT1#</t>
+  </si>
+  <si>
     <t>#IM.MI11DEN1#</t>
+  </si>
+  <si>
+    <t>#IM.IM11NUMT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM11NUMT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM11DENT3#</t>
+  </si>
+  <si>
+    <t>#IM.IM11NUMT3#</t>
+  </si>
+  <si>
+    <t>#IM.IM12DENT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM12NUMT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM12DENT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM12NUMT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM13DENT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM13NUMT1#</t>
+  </si>
+  <si>
+    <t>#IM.IM13DENT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM13NUMT2#</t>
+  </si>
+  <si>
+    <t>#IM.IM13DENT3#</t>
+  </si>
+  <si>
+    <t>#IM.IM13NUMT3#</t>
+  </si>
+  <si>
+    <t>#IM.IM13DENT4#</t>
+  </si>
+  <si>
+    <t>#IM.IM13NUMT4#</t>
+  </si>
+  <si>
+    <t>#IM.IM13DENT5#</t>
+  </si>
+  <si>
+    <t>#IM.IM13NUMT5#</t>
+  </si>
+  <si>
+    <t>#IM.VLDENT1#</t>
+  </si>
+  <si>
+    <t>#IM.VL1DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL2DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL3DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL4DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VLNUM1#</t>
+  </si>
+  <si>
+    <t>#IM.VL1NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL2NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL3NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL4NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VLDENT2#</t>
+  </si>
+  <si>
+    <t>#IM.VL5DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL6DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL7DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL8DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VLNUMT2#</t>
+  </si>
+  <si>
+    <t>#IM.VL5NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL6NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL7NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL8NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VLDENT3#</t>
+  </si>
+  <si>
+    <t>#IM.VL9DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL10DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL11DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VL12DEN#</t>
+  </si>
+  <si>
+    <t>#IM.VLNUMT3#</t>
+  </si>
+  <si>
+    <t>#IM.VL9NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL10NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL11NUM#</t>
+  </si>
+  <si>
+    <t>#IM.VL12NUM#</t>
+  </si>
+  <si>
+    <t>#IM.APSS1DEN#</t>
+  </si>
+  <si>
+    <t>#IM.APSS1NUM#</t>
+  </si>
+  <si>
+    <t>#IM.APSS2DEN#</t>
+  </si>
+  <si>
+    <t>#IM.APSS2NUM#</t>
+  </si>
+  <si>
+    <t>#IM.PWVL1DEN#</t>
+  </si>
+  <si>
+    <t>#IM.PWVL1NUM#</t>
   </si>
 </sst>
 </file>
@@ -2857,14 +3048,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="dd\-mm\-yyyy;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="dd\-mm\-yyyy;@"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3027,6 +3218,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3034,9 +3233,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3045,42 +3266,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3096,7 +3281,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3117,14 +3317,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -3132,32 +3324,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3193,7 +3377,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="54">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3333,7 +3517,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3345,13 +3541,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3363,37 +3559,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3405,31 +3589,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3441,73 +3607,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3885,66 +3985,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -3968,8 +4012,49 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3977,148 +4062,163 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="27" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="33" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4171,7 +4271,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -4574,10 +4674,10 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="20" borderId="25" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="8" fillId="20" borderId="25" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="20" borderId="17" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="8" fillId="20" borderId="17" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="20" borderId="29" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4598,7 +4698,7 @@
     <xf numFmtId="0" fontId="18" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="20" borderId="25" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="6" fillId="20" borderId="25" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -4609,14 +4709,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="20" borderId="20" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="7" fillId="20" borderId="20" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="18" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="20" borderId="21" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="7" fillId="20" borderId="21" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -4631,7 +4731,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="20" borderId="23" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="7" fillId="20" borderId="23" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -4678,7 +4778,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="20" borderId="25" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="7" fillId="20" borderId="25" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -5262,7 +5362,7 @@
   </sheetPr>
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScalePageLayoutView="90" topLeftCell="A47" workbookViewId="0">
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
@@ -6851,7 +6951,7 @@
         <v>184</v>
       </c>
       <c r="G50" s="176" t="e">
-        <f>E50/F50</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="H50" s="161"/>
@@ -7176,7 +7276,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -7538,8 +7638,8 @@
   <sheetPr/>
   <dimension ref="A1:GJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC3" workbookViewId="0">
-      <selection activeCell="AK13" sqref="AK13"/>
+    <sheetView tabSelected="1" topLeftCell="GE3" workbookViewId="0">
+      <selection activeCell="GL10" sqref="GL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -8791,379 +8891,379 @@
         <v>307</v>
       </c>
       <c r="BA9" s="24" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="BB9" s="24" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="BC9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="BD9" s="13" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="BE9" s="13" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="BF9" s="13" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="BG9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="BH9" s="13" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="BI9" s="13" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="BJ9" s="13" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="BK9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="BL9" s="13" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="BM9" s="13" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="BN9" s="13" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="BO9" s="18" t="s">
         <v>295</v>
       </c>
       <c r="BP9" s="24" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="BQ9" s="24" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="BR9" s="24" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="BS9" s="18" t="s">
         <v>295</v>
       </c>
       <c r="BT9" s="24" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="BU9" s="24" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="BV9" s="24" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="BW9" s="18" t="s">
         <v>295</v>
       </c>
       <c r="BX9" s="24" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="BY9" s="24" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="BZ9" s="24" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="CA9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="CB9" s="13" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="CC9" s="13" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="CD9" s="13" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="CE9" s="13" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="CF9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="CG9" s="13" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="CH9" s="13" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="CI9" s="13" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="CJ9" s="13" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="CK9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="CL9" s="13" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="CM9" s="13" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="CN9" s="13" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="CO9" s="13" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="CP9" s="29" t="s">
         <v>295</v>
       </c>
       <c r="CQ9" s="24" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="CR9" s="24" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="CS9" s="29" t="s">
         <v>295</v>
       </c>
       <c r="CT9" s="24" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="CU9" s="24" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="CV9" s="29" t="s">
         <v>295</v>
       </c>
       <c r="CW9" s="24" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="CX9" s="24" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="CY9" s="33" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="CZ9" s="33" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="DA9" s="33" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="DB9" s="33" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="DC9" s="33" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="DD9" s="33" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="DE9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="DF9" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="DG9" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="DH9" s="13" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="DI9" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="DJ9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="DK9" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="DL9" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="DM9" s="13" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="DN9" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="DO9" s="12" t="s">
         <v>295</v>
       </c>
       <c r="DP9" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="DQ9" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="DR9" s="13" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="DS9" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="DT9" s="29" t="s">
         <v>295</v>
       </c>
       <c r="DU9" s="24" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="DV9" s="24" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="DW9" s="29" t="s">
         <v>295</v>
       </c>
       <c r="DX9" s="24" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="DY9" s="24" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="DZ9" s="29" t="s">
         <v>295</v>
       </c>
       <c r="EA9" s="24" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="EB9" s="24" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="EC9" s="33" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="ED9" s="33" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="EE9" s="33" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="EF9" s="18" t="s">
         <v>295</v>
       </c>
       <c r="EG9" s="24" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="EH9" s="24" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="EI9" s="24" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="EJ9" s="18" t="s">
         <v>295</v>
       </c>
       <c r="EK9" s="24" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="EL9" s="24" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="EM9" s="24" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="EN9" s="18" t="s">
         <v>295</v>
       </c>
       <c r="EO9" s="24" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="EP9" s="24" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="EQ9" s="41" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="ER9" s="42" t="s">
         <v>295</v>
       </c>
       <c r="ES9" s="43" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="ET9" s="43" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="EU9" s="43" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="EV9" s="43" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="EW9" s="43" t="s">
         <v>295</v>
       </c>
       <c r="EX9" s="43" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="EY9" s="43" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="EZ9" s="43" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="FA9" s="43" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="FB9" s="43" t="s">
         <v>295</v>
       </c>
       <c r="FC9" s="43" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="FD9" s="43" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="FE9" s="43" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="FF9" s="43" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="FG9" s="43" t="s">
         <v>295</v>
       </c>
       <c r="FH9" s="43" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="FI9" s="43" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="FJ9" s="43" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="FK9" s="43" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="FL9" s="43" t="s">
         <v>295</v>
       </c>
       <c r="FM9" s="43" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="FN9" s="43" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="FO9" s="43" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="FP9" s="43" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="FQ9" s="43" t="s">
         <v>295</v>
       </c>
       <c r="FR9" s="43" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="FS9" s="43" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="FT9" s="43" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="FU9" s="43" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="FV9" s="40"/>
       <c r="FW9" s="40"/>
@@ -9172,34 +9272,43 @@
       <c r="FZ9" s="40"/>
       <c r="GA9" s="40"/>
       <c r="GB9" s="33" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="GC9" s="33" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="GD9" s="33" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="GE9" s="13" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="GF9" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="GG9" s="13" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="GH9" s="53" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="GI9" s="53" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="GJ9" s="53" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
-    <row r="10" spans="4:192">
+    <row r="10" spans="1:192">
+      <c r="A10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" t="s">
+        <v>353</v>
+      </c>
+      <c r="C10" t="s">
+        <v>354</v>
+      </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
@@ -9209,6 +9318,9 @@
       <c r="F10" t="s">
         <v>42</v>
       </c>
+      <c r="G10" t="s">
+        <v>355</v>
+      </c>
       <c r="H10" t="s">
         <v>23</v>
       </c>
@@ -9220,7 +9332,7 @@
       </c>
       <c r="K10" s="15" t="e">
         <f>G10/C10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L10" s="15" t="e">
         <f>H10/D10</f>
@@ -9234,6 +9346,9 @@
         <f>J10/F10</f>
         <v>#VALUE!</v>
       </c>
+      <c r="O10" t="s">
+        <v>356</v>
+      </c>
       <c r="P10" t="s">
         <v>28</v>
       </c>
@@ -9243,6 +9358,9 @@
       <c r="R10" t="s">
         <v>46</v>
       </c>
+      <c r="S10" t="s">
+        <v>357</v>
+      </c>
       <c r="T10" t="s">
         <v>27</v>
       </c>
@@ -9254,7 +9372,7 @@
       </c>
       <c r="W10" s="15" t="e">
         <f>S10/O10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X10" s="15" t="e">
         <f>T10/P10</f>
@@ -9268,8 +9386,11 @@
         <f>V10/R10</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AA10" t="s">
+        <v>358</v>
+      </c>
       <c r="AB10" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="AC10" t="s">
         <v>60</v>
@@ -9280,6 +9401,9 @@
       <c r="AE10" t="s">
         <v>72</v>
       </c>
+      <c r="AF10" t="s">
+        <v>360</v>
+      </c>
       <c r="AG10" t="s">
         <v>50</v>
       </c>
@@ -9289,12 +9413,15 @@
       <c r="AI10" t="s">
         <v>67</v>
       </c>
+      <c r="AJ10" t="s">
+        <v>361</v>
+      </c>
       <c r="AK10" t="s">
         <v>71</v>
       </c>
       <c r="AL10" s="15" t="e">
         <f>(AJ10+AF10)/AA10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AM10" s="15" t="e">
         <f>AG10/AB10</f>
@@ -9312,193 +9439,493 @@
         <f>AC10/AH10</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AQ10" t="s">
+        <v>362</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>363</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>63</v>
+      </c>
       <c r="AY10" s="15" t="e">
         <f>AU10/AQ10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AZ10" s="15" t="e">
         <f>AV10/AR10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BA10" s="15" t="e">
         <f>AW10/AS10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BB10" s="15" t="e">
         <f>AX10/AT10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>364</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE10" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>96</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>365</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>95</v>
       </c>
       <c r="BK10" s="15" t="e">
         <f>BG10/BC10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BL10" s="15" t="e">
         <f>BH10/BD10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BM10" s="15" t="e">
         <f>BI10/BE10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BN10" s="15" t="e">
         <f>BJ10/BF10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BO10" t="s">
+        <v>366</v>
+      </c>
+      <c r="BP10" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ10" t="s">
+        <v>92</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>100</v>
+      </c>
+      <c r="BS10" t="s">
+        <v>367</v>
+      </c>
+      <c r="BT10" t="s">
+        <v>83</v>
+      </c>
+      <c r="BU10" t="s">
+        <v>91</v>
+      </c>
+      <c r="BV10" t="s">
+        <v>99</v>
       </c>
       <c r="BW10" s="15" t="e">
         <f>BS10/BO10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BX10" s="15" t="e">
         <f>BT10/BP10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BY10" s="15" t="e">
         <f>BU10/BQ10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BZ10" s="15" t="e">
         <f>BV10/BR10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="CA10" t="s">
+        <v>368</v>
+      </c>
+      <c r="CB10" t="s">
+        <v>105</v>
+      </c>
+      <c r="CC10" t="s">
+        <v>125</v>
+      </c>
+      <c r="CD10" t="s">
+        <v>129</v>
+      </c>
+      <c r="CE10" t="s">
+        <v>133</v>
+      </c>
+      <c r="CF10" t="s">
+        <v>369</v>
+      </c>
+      <c r="CG10" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH10" t="s">
+        <v>124</v>
+      </c>
+      <c r="CI10" t="s">
+        <v>128</v>
+      </c>
+      <c r="CJ10" t="s">
+        <v>132</v>
       </c>
       <c r="CK10" s="15" t="e">
         <f>CF10/CA10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="CL10" s="15" t="e">
         <f>CG10/CB10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="CM10" s="15" t="e">
         <f>CH10/CC10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="CN10" s="15" t="e">
         <f>CI10/CD10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="CO10" s="15" t="e">
         <f>CJ10/CE10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="CP10" t="s">
+        <v>370</v>
+      </c>
+      <c r="CQ10" t="s">
+        <v>117</v>
+      </c>
+      <c r="CR10" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS10" t="s">
+        <v>371</v>
+      </c>
+      <c r="CT10" t="s">
+        <v>116</v>
+      </c>
+      <c r="CU10" t="s">
+        <v>152</v>
       </c>
       <c r="CV10" s="15" t="e">
         <f>CS10/CP10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="CW10" s="15" t="e">
         <f>CT10/CQ10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="CX10" s="15" t="e">
         <f>CU10/CR10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="CY10" t="s">
+        <v>162</v>
+      </c>
+      <c r="CZ10" t="s">
+        <v>161</v>
+      </c>
+      <c r="DA10" t="s">
+        <v>166</v>
+      </c>
+      <c r="DB10" t="s">
+        <v>165</v>
       </c>
       <c r="DC10" s="15" t="e">
         <f>CZ10/CY10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="DD10" s="15" t="e">
         <f>DB10/DA10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="DE10" t="s">
+        <v>372</v>
+      </c>
+      <c r="DF10" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG10" t="s">
+        <v>137</v>
+      </c>
+      <c r="DH10" t="s">
+        <v>141</v>
+      </c>
+      <c r="DI10" t="s">
+        <v>145</v>
+      </c>
+      <c r="DJ10" t="s">
+        <v>373</v>
+      </c>
+      <c r="DK10" t="s">
+        <v>108</v>
+      </c>
+      <c r="DL10" t="s">
+        <v>136</v>
+      </c>
+      <c r="DM10" t="s">
+        <v>140</v>
+      </c>
+      <c r="DN10" t="s">
+        <v>144</v>
       </c>
       <c r="DO10" s="15" t="e">
         <f>DJ10/DE10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="DP10" s="15" t="e">
         <f>DK10/DF10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="DQ10" s="15" t="e">
         <f>DL10/DG10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="DR10" s="15" t="e">
         <f>DM10/DH10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="DS10" s="15" t="e">
         <f>DN10/DI10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="DT10" t="s">
+        <v>374</v>
+      </c>
+      <c r="DU10" t="s">
+        <v>121</v>
+      </c>
+      <c r="DV10" t="s">
+        <v>157</v>
+      </c>
+      <c r="DW10" t="s">
+        <v>375</v>
+      </c>
+      <c r="DX10" t="s">
+        <v>120</v>
+      </c>
+      <c r="DY10" t="s">
+        <v>156</v>
       </c>
       <c r="DZ10" s="15" t="e">
         <f>DW10/DT10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="EA10" s="15" t="e">
         <f>DX10/DU10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="EB10" s="15" t="e">
         <f>DY10/DV10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="EC10" t="s">
+        <v>170</v>
+      </c>
+      <c r="ED10" t="s">
+        <v>169</v>
       </c>
       <c r="EE10" s="15" t="e">
         <f>ED10/EC10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="EF10" t="s">
+        <v>376</v>
+      </c>
+      <c r="EG10" t="s">
+        <v>113</v>
+      </c>
+      <c r="EH10" t="s">
+        <v>149</v>
+      </c>
+      <c r="EI10" t="s">
+        <v>174</v>
+      </c>
+      <c r="EJ10" t="s">
+        <v>377</v>
+      </c>
+      <c r="EK10" t="s">
+        <v>112</v>
+      </c>
+      <c r="EL10" t="s">
+        <v>148</v>
+      </c>
+      <c r="EM10" t="s">
+        <v>173</v>
       </c>
       <c r="EN10" s="15" t="e">
         <f>EJ10/EF10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="EO10" s="15" t="e">
         <f>EK10/EG10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="EP10" s="15" t="e">
         <f>EL10/EH10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="EQ10" s="15" t="e">
         <f>EM10/EI10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="ER10" s="6"/>
-      <c r="ES10" s="6"/>
-      <c r="ET10" s="6"/>
-      <c r="EU10" s="6"/>
-      <c r="EV10" s="6"/>
-      <c r="EW10" s="6"/>
-      <c r="EX10" s="6"/>
-      <c r="EY10" s="6"/>
-      <c r="EZ10" s="6"/>
-      <c r="FA10" s="6"/>
-      <c r="FB10" s="6"/>
-      <c r="FC10" s="6"/>
-      <c r="FD10" s="6"/>
-      <c r="FE10" s="6"/>
-      <c r="FF10" s="6"/>
-      <c r="FG10" s="6"/>
-      <c r="FH10" s="6"/>
-      <c r="FI10" s="6"/>
-      <c r="FJ10" s="6"/>
-      <c r="FK10" s="6"/>
-      <c r="FL10" s="6"/>
-      <c r="FM10" s="6"/>
-      <c r="FN10" s="6"/>
-      <c r="FO10" s="6"/>
-      <c r="FP10" s="6"/>
-      <c r="FQ10" s="6"/>
-      <c r="FR10" s="6"/>
-      <c r="FS10" s="6"/>
-      <c r="FT10" s="6"/>
-      <c r="FU10" s="6"/>
-      <c r="FV10" s="6"/>
-      <c r="FW10" s="6"/>
-      <c r="FX10" s="6"/>
-      <c r="FY10" s="6"/>
-      <c r="FZ10" s="6"/>
-      <c r="GA10" s="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="ER10" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="ES10" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="ET10" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="EU10" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="EV10" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="EW10" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="EX10" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="EY10" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="EZ10" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="FA10" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="FB10" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="FC10" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="FD10" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="FE10" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="FF10" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="FG10" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="FH10" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="FI10" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="FJ10" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="FK10" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="FL10" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="FM10" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="FN10" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="FO10" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="FP10" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="FQ10" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="FR10" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="FS10" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="FT10" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="FU10" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="FV10" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="FW10" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="FX10" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="FY10" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="FZ10" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="GA10" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="GB10" t="s">
+        <v>180</v>
+      </c>
+      <c r="GC10" t="s">
+        <v>179</v>
+      </c>
       <c r="GD10" s="15" t="e">
         <f>GC10/GB10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="GE10" t="s">
+        <v>184</v>
+      </c>
+      <c r="GF10" t="s">
+        <v>183</v>
       </c>
       <c r="GG10" s="15" t="e">
         <f>GF10/GE10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="GH10" t="s">
+        <v>188</v>
+      </c>
+      <c r="GI10" t="s">
+        <v>187</v>
       </c>
       <c r="GJ10" s="15" t="e">
         <f>GI10/GH10</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>